<commit_message>
Updated commit with 2019 data
</commit_message>
<xml_diff>
--- a/raw-data/WIR19_tab07.xlsx
+++ b/raw-data/WIR19_tab07.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\fdi_paper\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD704C0F-4384-476A-9BE9-4A1395A813B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1AC0EB-26BD-45C2-8D30-2FE97C7DD0EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -564,13 +564,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
     <col min="31" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="6" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" s="6" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>34</v>
       </c>
@@ -671,8 +671,11 @@
       <c r="AD1" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="AE1" s="6">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -763,8 +766,11 @@
       <c r="AD2" s="2">
         <v>25</v>
       </c>
+      <c r="AE2" s="1">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
@@ -855,8 +861,11 @@
       <c r="AD3" s="2">
         <v>100</v>
       </c>
+      <c r="AE3" s="1">
+        <v>79</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -947,8 +956,11 @@
       <c r="AD4" s="2">
         <v>126</v>
       </c>
+      <c r="AE4" s="1">
+        <v>155</v>
+      </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1039,8 +1051,11 @@
       <c r="AD5" s="2">
         <v>106</v>
       </c>
+      <c r="AE5" s="1">
+        <v>131</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1130,11 +1145,14 @@
       </c>
       <c r="AD6" s="2">
         <v>50</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF2">
-    <sortCondition ref="A68:A7"/>
+    <sortCondition ref="A7:A68"/>
   </sortState>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
@@ -1143,12 +1161,85 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <OriginalVersionID xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <ShortTitle xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <iddfa39abe6d4bbaa511b4aebbac8986 xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iddfa39abe6d4bbaa511b4aebbac8986>
+    <SalesNo xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <PublicationLinkId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <ISSN xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <ImagePathWhatsNew xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <Price xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <ImagePath xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <ReferenceItemId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <PublishDate xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">2019-06-11T22:00:00+00:00</PublishDate>
+    <ImagePathFlagship xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <p60be10af7c941a2b23bb5f20c154691 xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">WIR Annex Table - Excel</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">acf1c80a-3951-4241-93d4-b41d338d4719</TermId>
+        </TermInfo>
+      </Terms>
+    </p60be10af7c941a2b23bb5f20c154691>
+    <MeetingId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <Level1 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <Level4 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <Symbol xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <Size xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <OfficialDescription xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <LanguageId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <ReferenceFilePath xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <MeetingLinkId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <SpanishDocument xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </SpanishDocument>
+    <TaxCatchAll xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
+      <Value>1591</Value>
+    </TaxCatchAll>
+    <h2eb479c36154a2480beda2299c6b6c5 xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h2eb479c36154a2480beda2299c6b6c5>
+    <MeetingTitle xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <ParentDocId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <DocumentCategory xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <Level2 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <Level5 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <LongDescription xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <TableOfContent xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <EnglishDocument xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </EnglishDocument>
+    <FrenchDocument xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </FrenchDocument>
+    <ReferenceDocId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <de7de01eec0e4047a039d74943be32af xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </de7de01eec0e4047a039d74943be32af>
+    <e21d6563779b4a0cac0804544e1eafba xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e21d6563779b4a0cac0804544e1eafba>
+    <UNCTADLanguage xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <DocTitle xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <DocumentLabel xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <Level3 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <NumberOfPages xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <OriginalLanguages xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <SubTitle xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <HighLights xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <Symbol2 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <ISBN xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
+    <IsMigrated xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">1</IsMigrated>
+    <D8Migrate xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">Yes</D8Migrate>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1629,91 +1720,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <OriginalVersionID xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <ShortTitle xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <iddfa39abe6d4bbaa511b4aebbac8986 xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iddfa39abe6d4bbaa511b4aebbac8986>
-    <SalesNo xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <PublicationLinkId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <ISSN xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <ImagePathWhatsNew xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <Price xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <ImagePath xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <ReferenceItemId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <PublishDate xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">2019-06-11T22:00:00+00:00</PublishDate>
-    <ImagePathFlagship xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <p60be10af7c941a2b23bb5f20c154691 xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">WIR Annex Table - Excel</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">acf1c80a-3951-4241-93d4-b41d338d4719</TermId>
-        </TermInfo>
-      </Terms>
-    </p60be10af7c941a2b23bb5f20c154691>
-    <MeetingId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <Level1 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <Level4 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <Symbol xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <Size xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <OfficialDescription xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <LanguageId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <ReferenceFilePath xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <MeetingLinkId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <SpanishDocument xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </SpanishDocument>
-    <TaxCatchAll xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
-      <Value>1591</Value>
-    </TaxCatchAll>
-    <h2eb479c36154a2480beda2299c6b6c5 xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h2eb479c36154a2480beda2299c6b6c5>
-    <MeetingTitle xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <ParentDocId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <DocumentCategory xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <Level2 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <Level5 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <LongDescription xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <TableOfContent xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <EnglishDocument xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </EnglishDocument>
-    <FrenchDocument xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </FrenchDocument>
-    <ReferenceDocId xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <de7de01eec0e4047a039d74943be32af xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </de7de01eec0e4047a039d74943be32af>
-    <e21d6563779b4a0cac0804544e1eafba xmlns="60ea8e68-6540-4627-bb4d-21f975742799">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e21d6563779b4a0cac0804544e1eafba>
-    <UNCTADLanguage xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <DocTitle xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <DocumentLabel xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <Level3 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <NumberOfPages xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <OriginalLanguages xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <SubTitle xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <HighLights xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <Symbol2 xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <ISBN xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f" xsi:nil="true"/>
-    <IsMigrated xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">1</IsMigrated>
-    <D8Migrate xmlns="2c0079cb-7e3b-4b14-9551-8f7730befe9f">Yes</D8Migrate>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF44D824-4DFC-4E33-B22D-E6F292FA8DF6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05D0308C-0CAC-4DA1-9BAD-4CB762EBFF20}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2c0079cb-7e3b-4b14-9551-8f7730befe9f"/>
+    <ds:schemaRef ds:uri="60ea8e68-6540-4627-bb4d-21f975742799"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1738,12 +1759,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05D0308C-0CAC-4DA1-9BAD-4CB762EBFF20}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF44D824-4DFC-4E33-B22D-E6F292FA8DF6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2c0079cb-7e3b-4b14-9551-8f7730befe9f"/>
-    <ds:schemaRef ds:uri="60ea8e68-6540-4627-bb4d-21f975742799"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>